<commit_message>
Notifikációs követelmény és egy szekvenciadiagram hozzáadása
- egy új követelmény a felhasználók értesítéséről
- egy szekvenciadiagram hozzáadása a kommentelés működéséről
- tervek részletesebb leírása
- use-case és osztálydiagram frissítése az új követelmények szerint
</commit_message>
<xml_diff>
--- a/specifikacio/misc/kovetelmenyek.xlsx
+++ b/specifikacio/misc/kovetelmenyek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gyakornok\Documents\GitHub\IntrendChan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gyakornok\Documents\GitHub\IntrendChan\specifikacio\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9677228-0E92-43FB-BB8F-896D81E0C395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4025C32D-6658-4648-BEA1-3E4BE9B236BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{4801AA99-5C8B-47E7-A2FF-FE8EFD27C4A9}"/>
+    <workbookView xWindow="5265" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{4801AA99-5C8B-47E7-A2FF-FE8EFD27C4A9}"/>
   </bookViews>
   <sheets>
     <sheet name="kovetelmenyek" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>A kommenteket lehet kronológikusan, vagy szavazat alapján rendezni</t>
+  </si>
+  <si>
+    <t>A felhasználó értesítést kap, ha szavazat vagy válasz érkezik egy kommentjére</t>
+  </si>
+  <si>
+    <t>Az értesítés addig aktív, amíg a felhasználó interkacióba nem lép vele</t>
   </si>
 </sst>
 </file>
@@ -457,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F539CB-F2D6-4B3D-848E-3D0684062EFB}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +685,30 @@
         <v>23</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>